<commit_message>
update the lagouSpider -> lagouX make it better
</commit_message>
<xml_diff>
--- a/lagou.xlsx
+++ b/lagou.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\张霄港\Desktop\hive\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7440"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2768" uniqueCount="1361">
   <si>
     <t>companyClass</t>
   </si>
@@ -4437,23 +4441,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -4468,26 +4481,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -4775,20 +4805,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I346"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4814,8 +4851,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -4843,8 +4880,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -4872,8 +4909,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -4901,8 +4938,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -4930,8 +4967,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -4959,8 +4996,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -4988,8 +5025,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -5017,8 +5054,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -5046,8 +5083,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -5075,8 +5112,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
@@ -5104,8 +5141,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -5133,8 +5170,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -5162,8 +5199,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -5191,8 +5228,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -5220,8 +5257,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -5249,8 +5286,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -5278,8 +5315,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -5307,8 +5344,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -5336,8 +5373,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -5365,8 +5402,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -5394,8 +5431,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -5423,8 +5460,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -5452,8 +5489,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -5481,8 +5518,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -5510,8 +5547,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
@@ -5539,8 +5576,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
@@ -5568,8 +5605,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="1" t="n">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
@@ -5597,8 +5634,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="1" t="n">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
@@ -5626,8 +5663,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="1" t="n">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
@@ -5655,8 +5692,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="1" t="n">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
@@ -5684,8 +5721,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="1" t="n">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
@@ -5713,8 +5750,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="1" t="n">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
@@ -5742,8 +5779,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="1" t="n">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
@@ -5771,8 +5808,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="1" t="n">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
@@ -5800,8 +5837,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="1" t="n">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
@@ -5829,8 +5866,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="1" t="n">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
@@ -5858,8 +5895,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="1" t="n">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
@@ -5887,8 +5924,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="1" t="n">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
@@ -5916,8 +5953,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="1" t="n">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
@@ -5945,8 +5982,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="1" t="n">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
@@ -5974,8 +6011,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="1" t="n">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
@@ -6003,8 +6040,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="1" t="n">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
@@ -6032,8 +6069,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="1" t="n">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
@@ -6061,8 +6098,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="1" t="n">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
@@ -6090,8 +6127,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="1" t="n">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
@@ -6119,8 +6156,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="1" t="n">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
@@ -6148,8 +6185,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="1" t="n">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
@@ -6177,8 +6214,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="1" t="n">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
@@ -6206,8 +6243,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="1" t="n">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
@@ -6235,8 +6272,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="1" t="n">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
@@ -6264,8 +6301,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="1" t="n">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
@@ -6293,8 +6330,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="1" t="n">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
@@ -6322,8 +6359,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="1" t="n">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" t="s">
@@ -6351,8 +6388,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="1" t="n">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" t="s">
@@ -6380,8 +6417,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="1" t="n">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" t="s">
@@ -6409,8 +6446,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="1" t="n">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" t="s">
@@ -6438,8 +6475,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="1" t="n">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" t="s">
@@ -6467,8 +6504,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="1" t="n">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" t="s">
@@ -6496,8 +6533,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="1" t="n">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" t="s">
@@ -6525,8 +6562,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="1" t="n">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" t="s">
@@ -6554,8 +6591,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="1" t="n">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" t="s">
@@ -6583,8 +6620,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="1" t="n">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
@@ -6612,8 +6649,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="1" t="n">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
@@ -6641,8 +6678,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="1" t="n">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" t="s">
@@ -6670,8 +6707,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="1" t="n">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
@@ -6699,8 +6736,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="1" t="n">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" t="s">
@@ -6728,8 +6765,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
-      <c r="A68" s="1" t="n">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
@@ -6757,8 +6794,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
-      <c r="A69" s="1" t="n">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" t="s">
@@ -6786,8 +6823,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
-      <c r="A70" s="1" t="n">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" t="s">
@@ -6815,8 +6852,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
-      <c r="A71" s="1" t="n">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" t="s">
@@ -6844,8 +6881,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="1" t="n">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" t="s">
@@ -6873,8 +6910,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="1" t="n">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" t="s">
@@ -6902,8 +6939,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="1" t="n">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" t="s">
@@ -6931,8 +6968,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
-      <c r="A75" s="1" t="n">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" t="s">
@@ -6960,8 +6997,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
-      <c r="A76" s="1" t="n">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" t="s">
@@ -6989,8 +7026,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
-      <c r="A77" s="1" t="n">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" t="s">
@@ -7018,8 +7055,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
-      <c r="A78" s="1" t="n">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" t="s">
@@ -7047,8 +7084,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
-      <c r="A79" s="1" t="n">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" t="s">
@@ -7076,8 +7113,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
-      <c r="A80" s="1" t="n">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80" t="s">
@@ -7105,8 +7142,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
-      <c r="A81" s="1" t="n">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" t="s">
@@ -7134,8 +7171,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
-      <c r="A82" s="1" t="n">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" t="s">
@@ -7163,8 +7200,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
-      <c r="A83" s="1" t="n">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" t="s">
@@ -7192,8 +7229,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="1" t="n">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" t="s">
@@ -7221,8 +7258,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
-      <c r="A85" s="1" t="n">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" t="s">
@@ -7250,8 +7287,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="1" t="n">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" t="s">
@@ -7279,8 +7316,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="1" t="n">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" t="s">
@@ -7308,8 +7345,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
-      <c r="A88" s="1" t="n">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" t="s">
@@ -7337,8 +7374,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
-      <c r="A89" s="1" t="n">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" t="s">
@@ -7366,8 +7403,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
-      <c r="A90" s="1" t="n">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" t="s">
@@ -7395,8 +7432,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
-      <c r="A91" s="1" t="n">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" t="s">
@@ -7424,8 +7461,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
-      <c r="A92" s="1" t="n">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" t="s">
@@ -7453,8 +7490,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
-      <c r="A93" s="1" t="n">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" t="s">
@@ -7482,8 +7519,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
-      <c r="A94" s="1" t="n">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" t="s">
@@ -7511,8 +7548,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
-      <c r="A95" s="1" t="n">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" t="s">
@@ -7540,8 +7577,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
-      <c r="A96" s="1" t="n">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96" t="s">
@@ -7569,8 +7606,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
-      <c r="A97" s="1" t="n">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" t="s">
@@ -7598,8 +7635,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
-      <c r="A98" s="1" t="n">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98" t="s">
@@ -7627,8 +7664,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
-      <c r="A99" s="1" t="n">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99" t="s">
@@ -7656,8 +7693,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
-      <c r="A100" s="1" t="n">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100" t="s">
@@ -7685,8 +7722,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
-      <c r="A101" s="1" t="n">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101" t="s">
@@ -7714,8 +7751,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
-      <c r="A102" s="1" t="n">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A102" s="1">
         <v>100</v>
       </c>
       <c r="B102" t="s">
@@ -7743,8 +7780,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
-      <c r="A103" s="1" t="n">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A103" s="1">
         <v>101</v>
       </c>
       <c r="B103" t="s">
@@ -7772,8 +7809,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
-      <c r="A104" s="1" t="n">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A104" s="1">
         <v>102</v>
       </c>
       <c r="B104" t="s">
@@ -7801,8 +7838,8 @@
         <v>494</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
-      <c r="A105" s="1" t="n">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A105" s="1">
         <v>103</v>
       </c>
       <c r="B105" t="s">
@@ -7830,8 +7867,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
-      <c r="A106" s="1" t="n">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A106" s="1">
         <v>104</v>
       </c>
       <c r="B106" t="s">
@@ -7859,8 +7896,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
-      <c r="A107" s="1" t="n">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A107" s="1">
         <v>105</v>
       </c>
       <c r="B107" t="s">
@@ -7888,8 +7925,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
-      <c r="A108" s="1" t="n">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A108" s="1">
         <v>106</v>
       </c>
       <c r="B108" t="s">
@@ -7917,8 +7954,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
-      <c r="A109" s="1" t="n">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A109" s="1">
         <v>107</v>
       </c>
       <c r="B109" t="s">
@@ -7946,8 +7983,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
-      <c r="A110" s="1" t="n">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A110" s="1">
         <v>108</v>
       </c>
       <c r="B110" t="s">
@@ -7975,8 +8012,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
-      <c r="A111" s="1" t="n">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A111" s="1">
         <v>109</v>
       </c>
       <c r="B111" t="s">
@@ -8004,8 +8041,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
-      <c r="A112" s="1" t="n">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A112" s="1">
         <v>110</v>
       </c>
       <c r="B112" t="s">
@@ -8033,8 +8070,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
-      <c r="A113" s="1" t="n">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A113" s="1">
         <v>111</v>
       </c>
       <c r="B113" t="s">
@@ -8062,8 +8099,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
-      <c r="A114" s="1" t="n">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A114" s="1">
         <v>112</v>
       </c>
       <c r="B114" t="s">
@@ -8091,8 +8128,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
-      <c r="A115" s="1" t="n">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A115" s="1">
         <v>113</v>
       </c>
       <c r="B115" t="s">
@@ -8120,8 +8157,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
-      <c r="A116" s="1" t="n">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A116" s="1">
         <v>114</v>
       </c>
       <c r="B116" t="s">
@@ -8149,8 +8186,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
-      <c r="A117" s="1" t="n">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A117" s="1">
         <v>115</v>
       </c>
       <c r="B117" t="s">
@@ -8178,8 +8215,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
-      <c r="A118" s="1" t="n">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A118" s="1">
         <v>116</v>
       </c>
       <c r="B118" t="s">
@@ -8207,8 +8244,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
-      <c r="A119" s="1" t="n">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A119" s="1">
         <v>117</v>
       </c>
       <c r="B119" t="s">
@@ -8236,8 +8273,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
-      <c r="A120" s="1" t="n">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A120" s="1">
         <v>118</v>
       </c>
       <c r="B120" t="s">
@@ -8265,8 +8302,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
-      <c r="A121" s="1" t="n">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A121" s="1">
         <v>119</v>
       </c>
       <c r="B121" t="s">
@@ -8294,8 +8331,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
-      <c r="A122" s="1" t="n">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A122" s="1">
         <v>120</v>
       </c>
       <c r="B122" t="s">
@@ -8323,8 +8360,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
-      <c r="A123" s="1" t="n">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A123" s="1">
         <v>121</v>
       </c>
       <c r="B123" t="s">
@@ -8352,8 +8389,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
-      <c r="A124" s="1" t="n">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A124" s="1">
         <v>122</v>
       </c>
       <c r="B124" t="s">
@@ -8381,8 +8418,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
-      <c r="A125" s="1" t="n">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A125" s="1">
         <v>123</v>
       </c>
       <c r="B125" t="s">
@@ -8410,8 +8447,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
-      <c r="A126" s="1" t="n">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A126" s="1">
         <v>124</v>
       </c>
       <c r="B126" t="s">
@@ -8439,8 +8476,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
-      <c r="A127" s="1" t="n">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A127" s="1">
         <v>125</v>
       </c>
       <c r="B127" t="s">
@@ -8468,8 +8505,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
-      <c r="A128" s="1" t="n">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A128" s="1">
         <v>126</v>
       </c>
       <c r="B128" t="s">
@@ -8497,8 +8534,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
-      <c r="A129" s="1" t="n">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A129" s="1">
         <v>127</v>
       </c>
       <c r="B129" t="s">
@@ -8526,8 +8563,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
-      <c r="A130" s="1" t="n">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A130" s="1">
         <v>128</v>
       </c>
       <c r="B130" t="s">
@@ -8555,8 +8592,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
-      <c r="A131" s="1" t="n">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A131" s="1">
         <v>129</v>
       </c>
       <c r="B131" t="s">
@@ -8584,8 +8621,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
-      <c r="A132" s="1" t="n">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A132" s="1">
         <v>130</v>
       </c>
       <c r="B132" t="s">
@@ -8613,8 +8650,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
-      <c r="A133" s="1" t="n">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A133" s="1">
         <v>131</v>
       </c>
       <c r="B133" t="s">
@@ -8642,8 +8679,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
-      <c r="A134" s="1" t="n">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A134" s="1">
         <v>132</v>
       </c>
       <c r="B134" t="s">
@@ -8671,8 +8708,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
-      <c r="A135" s="1" t="n">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A135" s="1">
         <v>133</v>
       </c>
       <c r="B135" t="s">
@@ -8700,8 +8737,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
-      <c r="A136" s="1" t="n">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A136" s="1">
         <v>134</v>
       </c>
       <c r="B136" t="s">
@@ -8729,8 +8766,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
-      <c r="A137" s="1" t="n">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A137" s="1">
         <v>135</v>
       </c>
       <c r="B137" t="s">
@@ -8758,8 +8795,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
-      <c r="A138" s="1" t="n">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A138" s="1">
         <v>136</v>
       </c>
       <c r="B138" t="s">
@@ -8787,8 +8824,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
-      <c r="A139" s="1" t="n">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A139" s="1">
         <v>137</v>
       </c>
       <c r="B139" t="s">
@@ -8816,8 +8853,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
-      <c r="A140" s="1" t="n">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A140" s="1">
         <v>138</v>
       </c>
       <c r="B140" t="s">
@@ -8845,8 +8882,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
-      <c r="A141" s="1" t="n">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A141" s="1">
         <v>139</v>
       </c>
       <c r="B141" t="s">
@@ -8874,8 +8911,8 @@
         <v>632</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
-      <c r="A142" s="1" t="n">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A142" s="1">
         <v>140</v>
       </c>
       <c r="B142" t="s">
@@ -8903,8 +8940,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
-      <c r="A143" s="1" t="n">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A143" s="1">
         <v>141</v>
       </c>
       <c r="B143" t="s">
@@ -8932,8 +8969,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
-      <c r="A144" s="1" t="n">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A144" s="1">
         <v>142</v>
       </c>
       <c r="B144" t="s">
@@ -8961,8 +8998,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
-      <c r="A145" s="1" t="n">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A145" s="1">
         <v>143</v>
       </c>
       <c r="B145" t="s">
@@ -8990,8 +9027,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
-      <c r="A146" s="1" t="n">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A146" s="1">
         <v>144</v>
       </c>
       <c r="B146" t="s">
@@ -9019,8 +9056,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
-      <c r="A147" s="1" t="n">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A147" s="1">
         <v>145</v>
       </c>
       <c r="B147" t="s">
@@ -9048,8 +9085,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
-      <c r="A148" s="1" t="n">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A148" s="1">
         <v>146</v>
       </c>
       <c r="B148" t="s">
@@ -9077,8 +9114,8 @@
         <v>494</v>
       </c>
     </row>
-    <row r="149" spans="1:9">
-      <c r="A149" s="1" t="n">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A149" s="1">
         <v>147</v>
       </c>
       <c r="B149" t="s">
@@ -9106,8 +9143,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
-      <c r="A150" s="1" t="n">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A150" s="1">
         <v>148</v>
       </c>
       <c r="B150" t="s">
@@ -9135,8 +9172,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
-      <c r="A151" s="1" t="n">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A151" s="1">
         <v>149</v>
       </c>
       <c r="B151" t="s">
@@ -9164,8 +9201,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
-      <c r="A152" s="1" t="n">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A152" s="1">
         <v>150</v>
       </c>
       <c r="B152" t="s">
@@ -9193,8 +9230,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
-      <c r="A153" s="1" t="n">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A153" s="1">
         <v>151</v>
       </c>
       <c r="B153" t="s">
@@ -9222,8 +9259,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
-      <c r="A154" s="1" t="n">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A154" s="1">
         <v>152</v>
       </c>
       <c r="B154" t="s">
@@ -9251,8 +9288,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
-      <c r="A155" s="1" t="n">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A155" s="1">
         <v>153</v>
       </c>
       <c r="B155" t="s">
@@ -9280,8 +9317,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:9">
-      <c r="A156" s="1" t="n">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A156" s="1">
         <v>154</v>
       </c>
       <c r="B156" t="s">
@@ -9309,8 +9346,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
-      <c r="A157" s="1" t="n">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A157" s="1">
         <v>155</v>
       </c>
       <c r="B157" t="s">
@@ -9338,8 +9375,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
-      <c r="A158" s="1" t="n">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A158" s="1">
         <v>156</v>
       </c>
       <c r="B158" t="s">
@@ -9367,8 +9404,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:9">
-      <c r="A159" s="1" t="n">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A159" s="1">
         <v>157</v>
       </c>
       <c r="B159" t="s">
@@ -9396,8 +9433,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
-      <c r="A160" s="1" t="n">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A160" s="1">
         <v>158</v>
       </c>
       <c r="B160" t="s">
@@ -9425,8 +9462,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
-      <c r="A161" s="1" t="n">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A161" s="1">
         <v>159</v>
       </c>
       <c r="B161" t="s">
@@ -9454,8 +9491,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
-      <c r="A162" s="1" t="n">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A162" s="1">
         <v>160</v>
       </c>
       <c r="B162" t="s">
@@ -9483,8 +9520,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
-      <c r="A163" s="1" t="n">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A163" s="1">
         <v>161</v>
       </c>
       <c r="B163" t="s">
@@ -9512,8 +9549,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
-      <c r="A164" s="1" t="n">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A164" s="1">
         <v>162</v>
       </c>
       <c r="B164" t="s">
@@ -9541,8 +9578,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
-      <c r="A165" s="1" t="n">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A165" s="1">
         <v>163</v>
       </c>
       <c r="B165" t="s">
@@ -9570,8 +9607,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
-      <c r="A166" s="1" t="n">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A166" s="1">
         <v>164</v>
       </c>
       <c r="B166" t="s">
@@ -9599,8 +9636,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="167" spans="1:9">
-      <c r="A167" s="1" t="n">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A167" s="1">
         <v>165</v>
       </c>
       <c r="B167" t="s">
@@ -9628,8 +9665,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:9">
-      <c r="A168" s="1" t="n">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A168" s="1">
         <v>166</v>
       </c>
       <c r="B168" t="s">
@@ -9657,8 +9694,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:9">
-      <c r="A169" s="1" t="n">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A169" s="1">
         <v>167</v>
       </c>
       <c r="B169" t="s">
@@ -9686,8 +9723,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="170" spans="1:9">
-      <c r="A170" s="1" t="n">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A170" s="1">
         <v>168</v>
       </c>
       <c r="B170" t="s">
@@ -9715,8 +9752,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:9">
-      <c r="A171" s="1" t="n">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A171" s="1">
         <v>169</v>
       </c>
       <c r="B171" t="s">
@@ -9744,8 +9781,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
-      <c r="A172" s="1" t="n">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A172" s="1">
         <v>170</v>
       </c>
       <c r="B172" t="s">
@@ -9773,8 +9810,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
-      <c r="A173" s="1" t="n">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A173" s="1">
         <v>171</v>
       </c>
       <c r="B173" t="s">
@@ -9802,8 +9839,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
-      <c r="A174" s="1" t="n">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A174" s="1">
         <v>172</v>
       </c>
       <c r="B174" t="s">
@@ -9831,8 +9868,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
-      <c r="A175" s="1" t="n">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A175" s="1">
         <v>173</v>
       </c>
       <c r="B175" t="s">
@@ -9860,8 +9897,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
-      <c r="A176" s="1" t="n">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A176" s="1">
         <v>174</v>
       </c>
       <c r="B176" t="s">
@@ -9889,8 +9926,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
-      <c r="A177" s="1" t="n">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A177" s="1">
         <v>175</v>
       </c>
       <c r="B177" t="s">
@@ -9918,8 +9955,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:9">
-      <c r="A178" s="1" t="n">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A178" s="1">
         <v>176</v>
       </c>
       <c r="B178" t="s">
@@ -9947,8 +9984,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:9">
-      <c r="A179" s="1" t="n">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A179" s="1">
         <v>177</v>
       </c>
       <c r="B179" t="s">
@@ -9976,8 +10013,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
-      <c r="A180" s="1" t="n">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A180" s="1">
         <v>178</v>
       </c>
       <c r="B180" t="s">
@@ -10005,8 +10042,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:9">
-      <c r="A181" s="1" t="n">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A181" s="1">
         <v>179</v>
       </c>
       <c r="B181" t="s">
@@ -10034,8 +10071,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="182" spans="1:9">
-      <c r="A182" s="1" t="n">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A182" s="1">
         <v>180</v>
       </c>
       <c r="B182" t="s">
@@ -10063,8 +10100,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:9">
-      <c r="A183" s="1" t="n">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A183" s="1">
         <v>181</v>
       </c>
       <c r="B183" t="s">
@@ -10092,8 +10129,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:9">
-      <c r="A184" s="1" t="n">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A184" s="1">
         <v>182</v>
       </c>
       <c r="B184" t="s">
@@ -10121,8 +10158,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="185" spans="1:9">
-      <c r="A185" s="1" t="n">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A185" s="1">
         <v>183</v>
       </c>
       <c r="B185" t="s">
@@ -10150,8 +10187,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="186" spans="1:9">
-      <c r="A186" s="1" t="n">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A186" s="1">
         <v>184</v>
       </c>
       <c r="B186" t="s">
@@ -10179,8 +10216,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:9">
-      <c r="A187" s="1" t="n">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A187" s="1">
         <v>185</v>
       </c>
       <c r="B187" t="s">
@@ -10208,8 +10245,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="188" spans="1:9">
-      <c r="A188" s="1" t="n">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A188" s="1">
         <v>186</v>
       </c>
       <c r="B188" t="s">
@@ -10237,8 +10274,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="189" spans="1:9">
-      <c r="A189" s="1" t="n">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A189" s="1">
         <v>187</v>
       </c>
       <c r="B189" t="s">
@@ -10266,8 +10303,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="190" spans="1:9">
-      <c r="A190" s="1" t="n">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A190" s="1">
         <v>188</v>
       </c>
       <c r="B190" t="s">
@@ -10295,8 +10332,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="191" spans="1:9">
-      <c r="A191" s="1" t="n">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A191" s="1">
         <v>189</v>
       </c>
       <c r="B191" t="s">
@@ -10324,8 +10361,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="192" spans="1:9">
-      <c r="A192" s="1" t="n">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A192" s="1">
         <v>190</v>
       </c>
       <c r="B192" t="s">
@@ -10353,8 +10390,8 @@
         <v>632</v>
       </c>
     </row>
-    <row r="193" spans="1:9">
-      <c r="A193" s="1" t="n">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A193" s="1">
         <v>191</v>
       </c>
       <c r="B193" t="s">
@@ -10382,8 +10419,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="194" spans="1:9">
-      <c r="A194" s="1" t="n">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A194" s="1">
         <v>192</v>
       </c>
       <c r="B194" t="s">
@@ -10411,8 +10448,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="195" spans="1:9">
-      <c r="A195" s="1" t="n">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A195" s="1">
         <v>193</v>
       </c>
       <c r="B195" t="s">
@@ -10440,8 +10477,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="196" spans="1:9">
-      <c r="A196" s="1" t="n">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A196" s="1">
         <v>194</v>
       </c>
       <c r="B196" t="s">
@@ -10469,8 +10506,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="197" spans="1:9">
-      <c r="A197" s="1" t="n">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A197" s="1">
         <v>195</v>
       </c>
       <c r="B197" t="s">
@@ -10498,8 +10535,8 @@
         <v>835</v>
       </c>
     </row>
-    <row r="198" spans="1:9">
-      <c r="A198" s="1" t="n">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A198" s="1">
         <v>196</v>
       </c>
       <c r="B198" t="s">
@@ -10527,8 +10564,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="199" spans="1:9">
-      <c r="A199" s="1" t="n">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A199" s="1">
         <v>197</v>
       </c>
       <c r="B199" t="s">
@@ -10556,8 +10593,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="200" spans="1:9">
-      <c r="A200" s="1" t="n">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A200" s="1">
         <v>198</v>
       </c>
       <c r="B200" t="s">
@@ -10585,8 +10622,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="201" spans="1:9">
-      <c r="A201" s="1" t="n">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A201" s="1">
         <v>199</v>
       </c>
       <c r="B201" t="s">
@@ -10614,8 +10651,8 @@
         <v>851</v>
       </c>
     </row>
-    <row r="202" spans="1:9">
-      <c r="A202" s="1" t="n">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A202" s="1">
         <v>200</v>
       </c>
       <c r="B202" t="s">
@@ -10643,8 +10680,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="203" spans="1:9">
-      <c r="A203" s="1" t="n">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A203" s="1">
         <v>201</v>
       </c>
       <c r="B203" t="s">
@@ -10672,8 +10709,8 @@
         <v>632</v>
       </c>
     </row>
-    <row r="204" spans="1:9">
-      <c r="A204" s="1" t="n">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A204" s="1">
         <v>202</v>
       </c>
       <c r="B204" t="s">
@@ -10701,8 +10738,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="205" spans="1:9">
-      <c r="A205" s="1" t="n">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A205" s="1">
         <v>203</v>
       </c>
       <c r="B205" t="s">
@@ -10730,8 +10767,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="206" spans="1:9">
-      <c r="A206" s="1" t="n">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A206" s="1">
         <v>204</v>
       </c>
       <c r="B206" t="s">
@@ -10759,8 +10796,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="207" spans="1:9">
-      <c r="A207" s="1" t="n">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A207" s="1">
         <v>205</v>
       </c>
       <c r="B207" t="s">
@@ -10788,8 +10825,8 @@
         <v>879</v>
       </c>
     </row>
-    <row r="208" spans="1:9">
-      <c r="A208" s="1" t="n">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A208" s="1">
         <v>206</v>
       </c>
       <c r="B208" t="s">
@@ -10817,8 +10854,8 @@
         <v>882</v>
       </c>
     </row>
-    <row r="209" spans="1:9">
-      <c r="A209" s="1" t="n">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A209" s="1">
         <v>207</v>
       </c>
       <c r="B209" t="s">
@@ -10846,8 +10883,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="210" spans="1:9">
-      <c r="A210" s="1" t="n">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A210" s="1">
         <v>208</v>
       </c>
       <c r="B210" t="s">
@@ -10875,8 +10912,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="211" spans="1:9">
-      <c r="A211" s="1" t="n">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A211" s="1">
         <v>209</v>
       </c>
       <c r="B211" t="s">
@@ -10904,8 +10941,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:9">
-      <c r="A212" s="1" t="n">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A212" s="1">
         <v>210</v>
       </c>
       <c r="B212" t="s">
@@ -10933,8 +10970,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="213" spans="1:9">
-      <c r="A213" s="1" t="n">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A213" s="1">
         <v>211</v>
       </c>
       <c r="B213" t="s">
@@ -10962,8 +10999,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="214" spans="1:9">
-      <c r="A214" s="1" t="n">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A214" s="1">
         <v>212</v>
       </c>
       <c r="B214" t="s">
@@ -10991,8 +11028,8 @@
         <v>903</v>
       </c>
     </row>
-    <row r="215" spans="1:9">
-      <c r="A215" s="1" t="n">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A215" s="1">
         <v>213</v>
       </c>
       <c r="B215" t="s">
@@ -11020,8 +11057,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="216" spans="1:9">
-      <c r="A216" s="1" t="n">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A216" s="1">
         <v>214</v>
       </c>
       <c r="B216" t="s">
@@ -11049,8 +11086,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="217" spans="1:9">
-      <c r="A217" s="1" t="n">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A217" s="1">
         <v>215</v>
       </c>
       <c r="B217" t="s">
@@ -11078,8 +11115,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="218" spans="1:9">
-      <c r="A218" s="1" t="n">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A218" s="1">
         <v>216</v>
       </c>
       <c r="B218" t="s">
@@ -11107,8 +11144,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="219" spans="1:9">
-      <c r="A219" s="1" t="n">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A219" s="1">
         <v>217</v>
       </c>
       <c r="B219" t="s">
@@ -11136,8 +11173,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="220" spans="1:9">
-      <c r="A220" s="1" t="n">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A220" s="1">
         <v>218</v>
       </c>
       <c r="B220" t="s">
@@ -11165,8 +11202,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="221" spans="1:9">
-      <c r="A221" s="1" t="n">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A221" s="1">
         <v>219</v>
       </c>
       <c r="B221" t="s">
@@ -11194,8 +11231,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="222" spans="1:9">
-      <c r="A222" s="1" t="n">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A222" s="1">
         <v>220</v>
       </c>
       <c r="B222" t="s">
@@ -11223,8 +11260,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="223" spans="1:9">
-      <c r="A223" s="1" t="n">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A223" s="1">
         <v>221</v>
       </c>
       <c r="B223" t="s">
@@ -11252,8 +11289,8 @@
         <v>940</v>
       </c>
     </row>
-    <row r="224" spans="1:9">
-      <c r="A224" s="1" t="n">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A224" s="1">
         <v>222</v>
       </c>
       <c r="B224" t="s">
@@ -11281,8 +11318,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="225" spans="1:9">
-      <c r="A225" s="1" t="n">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A225" s="1">
         <v>223</v>
       </c>
       <c r="B225" t="s">
@@ -11310,8 +11347,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="226" spans="1:9">
-      <c r="A226" s="1" t="n">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A226" s="1">
         <v>224</v>
       </c>
       <c r="B226" t="s">
@@ -11339,8 +11376,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="227" spans="1:9">
-      <c r="A227" s="1" t="n">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A227" s="1">
         <v>225</v>
       </c>
       <c r="B227" t="s">
@@ -11368,8 +11405,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="228" spans="1:9">
-      <c r="A228" s="1" t="n">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A228" s="1">
         <v>226</v>
       </c>
       <c r="B228" t="s">
@@ -11397,8 +11434,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="229" spans="1:9">
-      <c r="A229" s="1" t="n">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A229" s="1">
         <v>227</v>
       </c>
       <c r="B229" t="s">
@@ -11426,8 +11463,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:9">
-      <c r="A230" s="1" t="n">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A230" s="1">
         <v>228</v>
       </c>
       <c r="B230" t="s">
@@ -11455,8 +11492,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="231" spans="1:9">
-      <c r="A231" s="1" t="n">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A231" s="1">
         <v>229</v>
       </c>
       <c r="B231" t="s">
@@ -11484,8 +11521,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="232" spans="1:9">
-      <c r="A232" s="1" t="n">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A232" s="1">
         <v>230</v>
       </c>
       <c r="B232" t="s">
@@ -11513,8 +11550,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="1:9">
-      <c r="A233" s="1" t="n">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A233" s="1">
         <v>231</v>
       </c>
       <c r="B233" t="s">
@@ -11542,8 +11579,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="234" spans="1:9">
-      <c r="A234" s="1" t="n">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A234" s="1">
         <v>232</v>
       </c>
       <c r="B234" t="s">
@@ -11571,8 +11608,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="235" spans="1:9">
-      <c r="A235" s="1" t="n">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A235" s="1">
         <v>233</v>
       </c>
       <c r="B235" t="s">
@@ -11600,8 +11637,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="236" spans="1:9">
-      <c r="A236" s="1" t="n">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A236" s="1">
         <v>234</v>
       </c>
       <c r="B236" t="s">
@@ -11629,8 +11666,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="237" spans="1:9">
-      <c r="A237" s="1" t="n">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A237" s="1">
         <v>235</v>
       </c>
       <c r="B237" t="s">
@@ -11658,8 +11695,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="238" spans="1:9">
-      <c r="A238" s="1" t="n">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A238" s="1">
         <v>236</v>
       </c>
       <c r="B238" t="s">
@@ -11687,8 +11724,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="239" spans="1:9">
-      <c r="A239" s="1" t="n">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A239" s="1">
         <v>237</v>
       </c>
       <c r="B239" t="s">
@@ -11716,8 +11753,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="240" spans="1:9">
-      <c r="A240" s="1" t="n">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A240" s="1">
         <v>238</v>
       </c>
       <c r="B240" t="s">
@@ -11745,8 +11782,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="241" spans="1:9">
-      <c r="A241" s="1" t="n">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A241" s="1">
         <v>239</v>
       </c>
       <c r="B241" t="s">
@@ -11774,8 +11811,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="242" spans="1:9">
-      <c r="A242" s="1" t="n">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A242" s="1">
         <v>240</v>
       </c>
       <c r="B242" t="s">
@@ -11803,8 +11840,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="243" spans="1:9">
-      <c r="A243" s="1" t="n">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A243" s="1">
         <v>241</v>
       </c>
       <c r="B243" t="s">
@@ -11832,8 +11869,8 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="244" spans="1:9">
-      <c r="A244" s="1" t="n">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A244" s="1">
         <v>242</v>
       </c>
       <c r="B244" t="s">
@@ -11861,8 +11898,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="245" spans="1:9">
-      <c r="A245" s="1" t="n">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A245" s="1">
         <v>243</v>
       </c>
       <c r="B245" t="s">
@@ -11890,8 +11927,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="246" spans="1:9">
-      <c r="A246" s="1" t="n">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A246" s="1">
         <v>244</v>
       </c>
       <c r="B246" t="s">
@@ -11919,8 +11956,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="247" spans="1:9">
-      <c r="A247" s="1" t="n">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A247" s="1">
         <v>245</v>
       </c>
       <c r="B247" t="s">
@@ -11948,8 +11985,8 @@
         <v>494</v>
       </c>
     </row>
-    <row r="248" spans="1:9">
-      <c r="A248" s="1" t="n">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A248" s="1">
         <v>246</v>
       </c>
       <c r="B248" t="s">
@@ -11977,8 +12014,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="249" spans="1:9">
-      <c r="A249" s="1" t="n">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A249" s="1">
         <v>247</v>
       </c>
       <c r="B249" t="s">
@@ -12006,8 +12043,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="250" spans="1:9">
-      <c r="A250" s="1" t="n">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A250" s="1">
         <v>248</v>
       </c>
       <c r="B250" t="s">
@@ -12035,8 +12072,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="251" spans="1:9">
-      <c r="A251" s="1" t="n">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A251" s="1">
         <v>249</v>
       </c>
       <c r="B251" t="s">
@@ -12064,8 +12101,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="252" spans="1:9">
-      <c r="A252" s="1" t="n">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A252" s="1">
         <v>250</v>
       </c>
       <c r="B252" t="s">
@@ -12093,8 +12130,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="253" spans="1:9">
-      <c r="A253" s="1" t="n">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A253" s="1">
         <v>251</v>
       </c>
       <c r="B253" t="s">
@@ -12122,8 +12159,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="254" spans="1:9">
-      <c r="A254" s="1" t="n">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A254" s="1">
         <v>252</v>
       </c>
       <c r="B254" t="s">
@@ -12151,8 +12188,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="255" spans="1:9">
-      <c r="A255" s="1" t="n">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A255" s="1">
         <v>253</v>
       </c>
       <c r="B255" t="s">
@@ -12180,8 +12217,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="256" spans="1:9">
-      <c r="A256" s="1" t="n">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A256" s="1">
         <v>254</v>
       </c>
       <c r="B256" t="s">
@@ -12209,8 +12246,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="257" spans="1:9">
-      <c r="A257" s="1" t="n">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A257" s="1">
         <v>255</v>
       </c>
       <c r="B257" t="s">
@@ -12238,8 +12275,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="258" spans="1:9">
-      <c r="A258" s="1" t="n">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A258" s="1">
         <v>256</v>
       </c>
       <c r="B258" t="s">
@@ -12267,8 +12304,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="259" spans="1:9">
-      <c r="A259" s="1" t="n">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A259" s="1">
         <v>257</v>
       </c>
       <c r="B259" t="s">
@@ -12296,8 +12333,8 @@
         <v>494</v>
       </c>
     </row>
-    <row r="260" spans="1:9">
-      <c r="A260" s="1" t="n">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A260" s="1">
         <v>258</v>
       </c>
       <c r="B260" t="s">
@@ -12325,8 +12362,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="261" spans="1:9">
-      <c r="A261" s="1" t="n">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A261" s="1">
         <v>259</v>
       </c>
       <c r="B261" t="s">
@@ -12354,8 +12391,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:9">
-      <c r="A262" s="1" t="n">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A262" s="1">
         <v>260</v>
       </c>
       <c r="B262" t="s">
@@ -12383,8 +12420,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="263" spans="1:9">
-      <c r="A263" s="1" t="n">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A263" s="1">
         <v>261</v>
       </c>
       <c r="B263" t="s">
@@ -12412,8 +12449,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:9">
-      <c r="A264" s="1" t="n">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A264" s="1">
         <v>262</v>
       </c>
       <c r="B264" t="s">
@@ -12441,8 +12478,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="265" spans="1:9">
-      <c r="A265" s="1" t="n">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A265" s="1">
         <v>263</v>
       </c>
       <c r="B265" t="s">
@@ -12470,8 +12507,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="266" spans="1:9">
-      <c r="A266" s="1" t="n">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A266" s="1">
         <v>264</v>
       </c>
       <c r="B266" t="s">
@@ -12499,8 +12536,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="267" spans="1:9">
-      <c r="A267" s="1" t="n">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A267" s="1">
         <v>265</v>
       </c>
       <c r="B267" t="s">
@@ -12528,8 +12565,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="268" spans="1:9">
-      <c r="A268" s="1" t="n">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A268" s="1">
         <v>266</v>
       </c>
       <c r="B268" t="s">
@@ -12557,8 +12594,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="269" spans="1:9">
-      <c r="A269" s="1" t="n">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A269" s="1">
         <v>267</v>
       </c>
       <c r="B269" t="s">
@@ -12586,8 +12623,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="270" spans="1:9">
-      <c r="A270" s="1" t="n">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A270" s="1">
         <v>268</v>
       </c>
       <c r="B270" t="s">
@@ -12615,8 +12652,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="271" spans="1:9">
-      <c r="A271" s="1" t="n">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A271" s="1">
         <v>269</v>
       </c>
       <c r="B271" t="s">
@@ -12644,8 +12681,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="272" spans="1:9">
-      <c r="A272" s="1" t="n">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A272" s="1">
         <v>270</v>
       </c>
       <c r="B272" t="s">
@@ -12673,8 +12710,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="273" spans="1:9">
-      <c r="A273" s="1" t="n">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A273" s="1">
         <v>271</v>
       </c>
       <c r="B273" t="s">
@@ -12702,8 +12739,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="274" spans="1:9">
-      <c r="A274" s="1" t="n">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A274" s="1">
         <v>272</v>
       </c>
       <c r="B274" t="s">
@@ -12731,8 +12768,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="275" spans="1:9">
-      <c r="A275" s="1" t="n">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A275" s="1">
         <v>273</v>
       </c>
       <c r="B275" t="s">
@@ -12760,8 +12797,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="276" spans="1:9">
-      <c r="A276" s="1" t="n">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A276" s="1">
         <v>274</v>
       </c>
       <c r="B276" t="s">
@@ -12789,8 +12826,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="277" spans="1:9">
-      <c r="A277" s="1" t="n">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A277" s="1">
         <v>275</v>
       </c>
       <c r="B277" t="s">
@@ -12818,8 +12855,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="278" spans="1:9">
-      <c r="A278" s="1" t="n">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A278" s="1">
         <v>276</v>
       </c>
       <c r="B278" t="s">
@@ -12847,8 +12884,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="279" spans="1:9">
-      <c r="A279" s="1" t="n">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A279" s="1">
         <v>277</v>
       </c>
       <c r="B279" t="s">
@@ -12876,8 +12913,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="280" spans="1:9">
-      <c r="A280" s="1" t="n">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A280" s="1">
         <v>278</v>
       </c>
       <c r="B280" t="s">
@@ -12905,8 +12942,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="281" spans="1:9">
-      <c r="A281" s="1" t="n">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A281" s="1">
         <v>279</v>
       </c>
       <c r="B281" t="s">
@@ -12934,8 +12971,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="282" spans="1:9">
-      <c r="A282" s="1" t="n">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A282" s="1">
         <v>280</v>
       </c>
       <c r="B282" t="s">
@@ -12963,8 +13000,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="283" spans="1:9">
-      <c r="A283" s="1" t="n">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A283" s="1">
         <v>281</v>
       </c>
       <c r="B283" t="s">
@@ -12992,8 +13029,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="284" spans="1:9">
-      <c r="A284" s="1" t="n">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A284" s="1">
         <v>282</v>
       </c>
       <c r="B284" t="s">
@@ -13021,8 +13058,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="285" spans="1:9">
-      <c r="A285" s="1" t="n">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A285" s="1">
         <v>283</v>
       </c>
       <c r="B285" t="s">
@@ -13050,8 +13087,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="286" spans="1:9">
-      <c r="A286" s="1" t="n">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A286" s="1">
         <v>284</v>
       </c>
       <c r="B286" t="s">
@@ -13079,8 +13116,8 @@
         <v>494</v>
       </c>
     </row>
-    <row r="287" spans="1:9">
-      <c r="A287" s="1" t="n">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A287" s="1">
         <v>285</v>
       </c>
       <c r="B287" t="s">
@@ -13108,8 +13145,8 @@
         <v>494</v>
       </c>
     </row>
-    <row r="288" spans="1:9">
-      <c r="A288" s="1" t="n">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A288" s="1">
         <v>286</v>
       </c>
       <c r="B288" t="s">
@@ -13137,8 +13174,8 @@
         <v>494</v>
       </c>
     </row>
-    <row r="289" spans="1:9">
-      <c r="A289" s="1" t="n">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A289" s="1">
         <v>287</v>
       </c>
       <c r="B289" t="s">
@@ -13166,8 +13203,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="290" spans="1:9">
-      <c r="A290" s="1" t="n">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A290" s="1">
         <v>288</v>
       </c>
       <c r="B290" t="s">
@@ -13195,8 +13232,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="291" spans="1:9">
-      <c r="A291" s="1" t="n">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A291" s="1">
         <v>289</v>
       </c>
       <c r="B291" t="s">
@@ -13224,8 +13261,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="292" spans="1:9">
-      <c r="A292" s="1" t="n">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A292" s="1">
         <v>290</v>
       </c>
       <c r="B292" t="s">
@@ -13253,8 +13290,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="293" spans="1:9">
-      <c r="A293" s="1" t="n">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A293" s="1">
         <v>291</v>
       </c>
       <c r="B293" t="s">
@@ -13282,8 +13319,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="294" spans="1:9">
-      <c r="A294" s="1" t="n">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A294" s="1">
         <v>292</v>
       </c>
       <c r="B294" t="s">
@@ -13311,8 +13348,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="295" spans="1:9">
-      <c r="A295" s="1" t="n">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A295" s="1">
         <v>293</v>
       </c>
       <c r="B295" t="s">
@@ -13340,8 +13377,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="296" spans="1:9">
-      <c r="A296" s="1" t="n">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A296" s="1">
         <v>294</v>
       </c>
       <c r="B296" t="s">
@@ -13369,8 +13406,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="297" spans="1:9">
-      <c r="A297" s="1" t="n">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A297" s="1">
         <v>295</v>
       </c>
       <c r="B297" t="s">
@@ -13398,8 +13435,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="298" spans="1:9">
-      <c r="A298" s="1" t="n">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A298" s="1">
         <v>296</v>
       </c>
       <c r="B298" t="s">
@@ -13427,8 +13464,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="299" spans="1:9">
-      <c r="A299" s="1" t="n">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A299" s="1">
         <v>297</v>
       </c>
       <c r="B299" t="s">
@@ -13456,8 +13493,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="300" spans="1:9">
-      <c r="A300" s="1" t="n">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A300" s="1">
         <v>298</v>
       </c>
       <c r="B300" t="s">
@@ -13485,8 +13522,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="301" spans="1:9">
-      <c r="A301" s="1" t="n">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A301" s="1">
         <v>299</v>
       </c>
       <c r="B301" t="s">
@@ -13514,8 +13551,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="302" spans="1:9">
-      <c r="A302" s="1" t="n">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A302" s="1">
         <v>300</v>
       </c>
       <c r="B302" t="s">
@@ -13543,8 +13580,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="303" spans="1:9">
-      <c r="A303" s="1" t="n">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A303" s="1">
         <v>301</v>
       </c>
       <c r="B303" t="s">
@@ -13572,8 +13609,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="304" spans="1:9">
-      <c r="A304" s="1" t="n">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A304" s="1">
         <v>302</v>
       </c>
       <c r="B304" t="s">
@@ -13601,8 +13638,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="305" spans="1:9">
-      <c r="A305" s="1" t="n">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A305" s="1">
         <v>303</v>
       </c>
       <c r="B305" t="s">
@@ -13630,8 +13667,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="306" spans="1:9">
-      <c r="A306" s="1" t="n">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A306" s="1">
         <v>304</v>
       </c>
       <c r="B306" t="s">
@@ -13659,8 +13696,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="307" spans="1:9">
-      <c r="A307" s="1" t="n">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A307" s="1">
         <v>305</v>
       </c>
       <c r="B307" t="s">
@@ -13688,8 +13725,8 @@
         <v>851</v>
       </c>
     </row>
-    <row r="308" spans="1:9">
-      <c r="A308" s="1" t="n">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A308" s="1">
         <v>306</v>
       </c>
       <c r="B308" t="s">
@@ -13717,8 +13754,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="309" spans="1:9">
-      <c r="A309" s="1" t="n">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A309" s="1">
         <v>307</v>
       </c>
       <c r="B309" t="s">
@@ -13746,8 +13783,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="310" spans="1:9">
-      <c r="A310" s="1" t="n">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A310" s="1">
         <v>308</v>
       </c>
       <c r="B310" t="s">
@@ -13775,8 +13812,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="311" spans="1:9">
-      <c r="A311" s="1" t="n">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A311" s="1">
         <v>309</v>
       </c>
       <c r="B311" t="s">
@@ -13804,8 +13841,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="312" spans="1:9">
-      <c r="A312" s="1" t="n">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A312" s="1">
         <v>310</v>
       </c>
       <c r="B312" t="s">
@@ -13833,8 +13870,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="313" spans="1:9">
-      <c r="A313" s="1" t="n">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A313" s="1">
         <v>311</v>
       </c>
       <c r="B313" t="s">
@@ -13862,8 +13899,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="314" spans="1:9">
-      <c r="A314" s="1" t="n">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A314" s="1">
         <v>312</v>
       </c>
       <c r="B314" t="s">
@@ -13891,8 +13928,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="315" spans="1:9">
-      <c r="A315" s="1" t="n">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A315" s="1">
         <v>313</v>
       </c>
       <c r="B315" t="s">
@@ -13920,8 +13957,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="316" spans="1:9">
-      <c r="A316" s="1" t="n">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A316" s="1">
         <v>314</v>
       </c>
       <c r="B316" t="s">
@@ -13949,8 +13986,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="317" spans="1:9">
-      <c r="A317" s="1" t="n">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A317" s="1">
         <v>315</v>
       </c>
       <c r="B317" t="s">
@@ -13978,8 +14015,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="318" spans="1:9">
-      <c r="A318" s="1" t="n">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A318" s="1">
         <v>316</v>
       </c>
       <c r="B318" t="s">
@@ -14007,8 +14044,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="319" spans="1:9">
-      <c r="A319" s="1" t="n">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A319" s="1">
         <v>317</v>
       </c>
       <c r="B319" t="s">
@@ -14036,8 +14073,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="320" spans="1:9">
-      <c r="A320" s="1" t="n">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A320" s="1">
         <v>318</v>
       </c>
       <c r="B320" t="s">
@@ -14065,8 +14102,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="321" spans="1:9">
-      <c r="A321" s="1" t="n">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A321" s="1">
         <v>319</v>
       </c>
       <c r="B321" t="s">
@@ -14094,8 +14131,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="322" spans="1:9">
-      <c r="A322" s="1" t="n">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A322" s="1">
         <v>320</v>
       </c>
       <c r="B322" t="s">
@@ -14123,8 +14160,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="323" spans="1:9">
-      <c r="A323" s="1" t="n">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A323" s="1">
         <v>321</v>
       </c>
       <c r="B323" t="s">
@@ -14152,8 +14189,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="324" spans="1:9">
-      <c r="A324" s="1" t="n">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A324" s="1">
         <v>322</v>
       </c>
       <c r="B324" t="s">
@@ -14181,8 +14218,8 @@
         <v>940</v>
       </c>
     </row>
-    <row r="325" spans="1:9">
-      <c r="A325" s="1" t="n">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A325" s="1">
         <v>323</v>
       </c>
       <c r="B325" t="s">
@@ -14210,8 +14247,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="326" spans="1:9">
-      <c r="A326" s="1" t="n">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A326" s="1">
         <v>324</v>
       </c>
       <c r="B326" t="s">
@@ -14239,8 +14276,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="327" spans="1:9">
-      <c r="A327" s="1" t="n">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A327" s="1">
         <v>325</v>
       </c>
       <c r="B327" t="s">
@@ -14268,8 +14305,8 @@
         <v>494</v>
       </c>
     </row>
-    <row r="328" spans="1:9">
-      <c r="A328" s="1" t="n">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A328" s="1">
         <v>326</v>
       </c>
       <c r="B328" t="s">
@@ -14297,8 +14334,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="329" spans="1:9">
-      <c r="A329" s="1" t="n">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A329" s="1">
         <v>327</v>
       </c>
       <c r="B329" t="s">
@@ -14326,8 +14363,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="330" spans="1:9">
-      <c r="A330" s="1" t="n">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A330" s="1">
         <v>328</v>
       </c>
       <c r="B330" t="s">
@@ -14355,8 +14392,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="331" spans="1:9">
-      <c r="A331" s="1" t="n">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A331" s="1">
         <v>329</v>
       </c>
       <c r="B331" t="s">
@@ -14384,8 +14421,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="332" spans="1:9">
-      <c r="A332" s="1" t="n">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A332" s="1">
         <v>330</v>
       </c>
       <c r="B332" t="s">
@@ -14413,8 +14450,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="333" spans="1:9">
-      <c r="A333" s="1" t="n">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A333" s="1">
         <v>331</v>
       </c>
       <c r="B333" t="s">
@@ -14442,8 +14479,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="334" spans="1:9">
-      <c r="A334" s="1" t="n">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A334" s="1">
         <v>332</v>
       </c>
       <c r="B334" t="s">
@@ -14471,8 +14508,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="335" spans="1:9">
-      <c r="A335" s="1" t="n">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A335" s="1">
         <v>333</v>
       </c>
       <c r="B335" t="s">
@@ -14500,8 +14537,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="336" spans="1:9">
-      <c r="A336" s="1" t="n">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A336" s="1">
         <v>334</v>
       </c>
       <c r="B336" t="s">
@@ -14529,8 +14566,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="337" spans="1:9">
-      <c r="A337" s="1" t="n">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A337" s="1">
         <v>335</v>
       </c>
       <c r="B337" t="s">
@@ -14558,8 +14595,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="338" spans="1:9">
-      <c r="A338" s="1" t="n">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A338" s="1">
         <v>336</v>
       </c>
       <c r="B338" t="s">
@@ -14587,8 +14624,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="339" spans="1:9">
-      <c r="A339" s="1" t="n">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A339" s="1">
         <v>337</v>
       </c>
       <c r="B339" t="s">
@@ -14616,8 +14653,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="340" spans="1:9">
-      <c r="A340" s="1" t="n">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A340" s="1">
         <v>338</v>
       </c>
       <c r="B340" t="s">
@@ -14645,8 +14682,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="341" spans="1:9">
-      <c r="A341" s="1" t="n">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A341" s="1">
         <v>339</v>
       </c>
       <c r="B341" t="s">
@@ -14674,8 +14711,8 @@
         <v>506</v>
       </c>
     </row>
-    <row r="342" spans="1:9">
-      <c r="A342" s="1" t="n">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A342" s="1">
         <v>340</v>
       </c>
       <c r="B342" t="s">
@@ -14703,8 +14740,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="343" spans="1:9">
-      <c r="A343" s="1" t="n">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A343" s="1">
         <v>341</v>
       </c>
       <c r="B343" t="s">
@@ -14732,8 +14769,8 @@
         <v>494</v>
       </c>
     </row>
-    <row r="344" spans="1:9">
-      <c r="A344" s="1" t="n">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A344" s="1">
         <v>342</v>
       </c>
       <c r="B344" t="s">
@@ -14761,8 +14798,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="345" spans="1:9">
-      <c r="A345" s="1" t="n">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A345" s="1">
         <v>343</v>
       </c>
       <c r="B345" t="s">
@@ -14790,8 +14827,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="346" spans="1:9">
-      <c r="A346" s="1" t="n">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A346" s="1">
         <v>344</v>
       </c>
       <c r="B346" t="s">
@@ -14820,6 +14857,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>